<commit_message>
Include the ratio for each energy metric
</commit_message>
<xml_diff>
--- a/round1983.xlsx
+++ b/round1983.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheun\Desktop\Green LLM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheun\Desktop\Green LLM\New folder\Green-LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B2ED9C-C25C-487E-BAC5-6E83549BC9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A954A68-D152-45DB-B50C-7AEF584FA666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Tasks</t>
   </si>
@@ -56,9 +56,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>All Tasks</t>
-  </si>
-  <si>
     <t>Power of laptop(watt)</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Mean Time Spent(Seconds)</t>
   </si>
   <si>
-    <t>Background energy consumption(kwh)</t>
-  </si>
-  <si>
     <t>Mean Python Memory Usage(kilobyte)</t>
   </si>
   <si>
@@ -150,6 +144,33 @@
   </si>
   <si>
     <t>Mean Python Runtime( millisec)</t>
+  </si>
+  <si>
+    <t>Coding energy consumption(kwh)</t>
+  </si>
+  <si>
+    <t>CEC-TTEC ratio</t>
+  </si>
+  <si>
+    <t>DEC-TTEC ratio</t>
+  </si>
+  <si>
+    <t>TEC-TTEC ratio</t>
+  </si>
+  <si>
+    <t>Energy spent on producing the insight (kwh)</t>
+  </si>
+  <si>
+    <t>Energy spent on addingg the missingg functionalities (kwh)</t>
+  </si>
+  <si>
+    <t>QEC - TTEC ratio</t>
+  </si>
+  <si>
+    <t>ESPI - TTEC ratio</t>
+  </si>
+  <si>
+    <t>ESAF - TTEC ratio</t>
   </si>
 </sst>
 </file>
@@ -202,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -219,6 +240,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -415,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -450,19 +472,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>444</v>
@@ -479,10 +498,6 @@
       <c r="F2">
         <v>2487</v>
       </c>
-      <c r="G2">
-        <f>SUM(C2:F2)</f>
-        <v>9082</v>
-      </c>
       <c r="L2">
         <v>4.0750000000000002</v>
       </c>
@@ -492,7 +507,7 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2">
         <f>$L$2*B2*$N$2</f>
@@ -514,15 +529,12 @@
         <f t="shared" si="0"/>
         <v>2.8151480854499999E-3</v>
       </c>
-      <c r="G3" s="5">
-        <f>SUM(B3:F3)</f>
-        <v>1.0782911404100001E-2</v>
-      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>68.680000000000007</v>
@@ -539,14 +551,10 @@
       <c r="F4">
         <v>1383.4</v>
       </c>
-      <c r="G4">
-        <f>AVERAGE(B4:F4)</f>
-        <v>502.7</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6">
         <f>8467/1000</f>
@@ -568,14 +576,11 @@
         <f>45096960/1000</f>
         <v>45096.959999999999</v>
       </c>
-      <c r="G5" s="6">
-        <f>AVERAGE(B5:F5)</f>
-        <v>23625.801799999997</v>
-      </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -592,14 +597,10 @@
       <c r="F6">
         <v>14</v>
       </c>
-      <c r="G6">
-        <f>AVERAGE(B6:F6)</f>
-        <v>14</v>
-      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -616,14 +617,10 @@
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="G7">
-        <f>AVERAGE(B7:F7)</f>
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>1.26</v>
@@ -640,15 +637,12 @@
       <c r="F8">
         <v>1.79</v>
       </c>
-      <c r="G8" s="7">
-        <f>AVERAGE(B8:F8)</f>
-        <v>1.7759999999999998</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
         <f>(B6+B7*(B5/(1024*1024)/$L$13))*(B4/1000)*B8*$N$2</f>
@@ -670,14 +664,11 @@
         <f>(F6+F7*(F5/(1024*1024)/$L$13))*(F4/1000)*F8*$N$2</f>
         <v>9.6411025369020103E-6</v>
       </c>
-      <c r="G9" s="2">
-        <f>SUM(B9:F9)</f>
-        <v>1.8277603396285907E-5</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <f>(B6+B7*(B5/(1024*1024)/$L$13) -$L$2)*B2*$L$28*$L$16*$N$2</f>
@@ -699,14 +690,11 @@
         <f>(F6+F7*(F5/(1024*1024)/$L$13) -$L$2)*F2*$L$28*$L$16*$N$2</f>
         <v>2.8844205763334436E-4</v>
       </c>
-      <c r="G10" s="2">
-        <f>SUM(B10:F10)</f>
-        <v>1.1041861958747006E-3</v>
-      </c>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4">
         <f>SUM(B3,B9,B10)</f>
@@ -728,189 +716,176 @@
         <f>SUM(F3,F9,F10)</f>
         <v>3.1132312456202465E-3</v>
       </c>
-      <c r="G11" s="4">
-        <f>SUM(B11:F11)</f>
-        <v>1.1905375203370986E-2</v>
-      </c>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <f>$L$25*B11</f>
-        <v>0.12029000592874926</v>
-      </c>
-      <c r="C12" s="5">
-        <f>$L$25*C11</f>
-        <v>0.60032808487741929</v>
-      </c>
-      <c r="D12" s="5">
-        <f>$L$25*D11</f>
-        <v>0.64011892265776404</v>
-      </c>
-      <c r="E12" s="5">
-        <f>$L$25*E11</f>
-        <v>0.54715822536797798</v>
-      </c>
-      <c r="F12" s="5">
-        <f>$L$25*F11</f>
-        <v>0.67557118029959351</v>
-      </c>
-      <c r="G12" s="9">
-        <f>SUM(B12:F12)</f>
-        <v>2.5834664191315042</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B12" s="12">
+        <f>B3/B11</f>
+        <v>0.90664781117725879</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" ref="C12:F12" si="1">C3/C11</f>
+        <v>0.90670557992692391</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="1"/>
+        <v>0.90598397306403378</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="1"/>
+        <v>0.90592745837593613</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="1"/>
+        <v>0.90425280467373059</v>
+      </c>
+      <c r="G12" s="9"/>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="12">
+        <f>B10/B11</f>
+        <v>9.2745093348324245E-2</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" ref="C13:F13" si="2">C10/C11</f>
+        <v>9.2766417143444427E-2</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="2"/>
+        <v>9.2834131720079316E-2</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="2"/>
+        <v>9.2742826279043358E-2</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="2"/>
+        <v>9.2650379903237254E-2</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="L13">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="12">
+        <f>B9/B11</f>
+        <v>6.0709547441705294E-4</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" ref="C14:F14" si="3">C9/C11</f>
+        <v>5.2800292963160061E-4</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="3"/>
+        <v>1.1818952158870102E-3</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="3"/>
+        <v>1.3297153450205225E-3</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="3"/>
+        <v>3.096815423032034E-3</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <f>$L$25*B11</f>
+        <v>0.12029000592874926</v>
+      </c>
+      <c r="C15" s="5">
+        <f>$L$25*C11</f>
+        <v>0.60032808487741929</v>
+      </c>
+      <c r="D15" s="5">
+        <f>$L$25*D11</f>
+        <v>0.64011892265776404</v>
+      </c>
+      <c r="E15" s="5">
+        <f>$L$25*E11</f>
+        <v>0.54715822536797798</v>
+      </c>
+      <c r="F15" s="5">
+        <f>$L$25*F11</f>
+        <v>0.67557118029959351</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
       <c r="H16" s="9"/>
       <c r="L16" s="10">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <f>SUM(B17:F17)</f>
-        <v>21</v>
-      </c>
-    </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8">
-        <v>0</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <f>AVERAGE(B18:F18)</f>
-        <v>0.2</v>
-      </c>
+      <c r="G18" s="8"/>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="11">
-        <f>(1+1+2)/3</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="11">
-        <f>(3+1+1)/3</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-      <c r="G19">
-        <f>SUM(B19:F19)</f>
-        <v>9</v>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
       </c>
       <c r="L19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
-        <f>(6.5% + 100% + 100%)/3</f>
-        <v>0.68833333333333335</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <f>AVERAGE(B20:F20)</f>
-        <v>0.53766666666666674</v>
-      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="J20" s="2"/>
       <c r="L20">
@@ -919,63 +894,50 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <f>(B17+B19)*$L$20</f>
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C21" s="9">
-        <f>(C17+C19)*$L$20</f>
-        <v>6.9666666666666655E-2</v>
-      </c>
-      <c r="D21">
-        <f>(D17+D19)*$L$20</f>
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="E21" s="9">
-        <f>(E17+E19)*$L$20</f>
-        <v>7.3333333333333334E-2</v>
-      </c>
-      <c r="F21">
-        <f t="shared" ref="F21" si="1">(F17+F19)*$L$20</f>
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="G21" s="9">
-        <f t="shared" ref="G21:G26" si="2">SUM(B21:F21)</f>
-        <v>0.32999999999999996</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9"/>
       <c r="L21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="6">
-        <f>C2*$L$36*(1-C18)</f>
-        <v>842.08</v>
-      </c>
-      <c r="D22" s="6">
-        <f>D2*$L$36*(1-D18)</f>
-        <v>897.18000000000006</v>
-      </c>
-      <c r="E22" s="6">
-        <f>E2*$L$36*(1-E18)</f>
-        <v>766.84</v>
-      </c>
-      <c r="F22" s="6">
-        <f>F2*$L$36*(1-F18)</f>
-        <v>945.06000000000006</v>
-      </c>
-      <c r="G22" s="6">
-        <f t="shared" si="2"/>
-        <v>3451.1600000000003</v>
-      </c>
+      <c r="C22" s="11">
+        <f>(1+1+2)/3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" s="11">
+        <f>(3+1+1)/3</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6"/>
       <c r="H22" s="8"/>
       <c r="L22">
         <v>50</v>
@@ -983,91 +945,80 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <f>($L$32+$L$34)*(D2*$L$28)</f>
-        <v>396.64800000000002</v>
-      </c>
-      <c r="E23" s="6">
-        <f>($L$32+$L$34)*(E2*$L$28)</f>
-        <v>339.024</v>
-      </c>
-      <c r="F23" s="6">
-        <f>($L$32+$L$34)*(F2*$L$28)</f>
-        <v>417.81600000000003</v>
-      </c>
-      <c r="G23" s="6">
-        <f t="shared" si="2"/>
-        <v>1153.4880000000001</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <f>(6.5% + 100% + 100%)/3</f>
+        <v>0.68833333333333335</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <f>(1-B20)*B2+B23</f>
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24" s="6">
-        <f>(1-D20)*D2+D23 - D22</f>
-        <v>1860.4680000000001</v>
-      </c>
-      <c r="E24" s="6">
-        <f>(1-E20)*E2+E23 - E22</f>
-        <v>201.12733333333324</v>
-      </c>
-      <c r="F24" s="6">
-        <f>(1-F20)*F2+F23 - F22</f>
-        <v>1959.7559999999999</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="2"/>
-        <v>4021.3513333333331</v>
-      </c>
+        <f>(B20+B22)*$L$20</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C24" s="9">
+        <f>(C20+C22)*$L$20</f>
+        <v>6.9666666666666655E-2</v>
+      </c>
+      <c r="D24">
+        <f>(D20+D22)*$L$20</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E24" s="9">
+        <f>(E20+E22)*$L$20</f>
+        <v>7.3333333333333334E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ref="F24" si="4">(F20+F22)*$L$20</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="L24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <f>B21+(B22+B24)*$L$2*$N$2</f>
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C25" s="5">
-        <f>C21+(C22+C24)*$L$2*$N$2</f>
-        <v>7.0619855206994653E-2</v>
-      </c>
-      <c r="D25" s="5">
-        <f>D21+(D22+D24)*$L$2*$N$2</f>
-        <v>9.1121506830536797E-2</v>
-      </c>
-      <c r="E25" s="5">
-        <f t="shared" ref="E25:F25" si="3">E21+(E22+E24)*$L$2*$N$2</f>
-        <v>7.4429019455251905E-2</v>
-      </c>
-      <c r="F25" s="5">
-        <f t="shared" si="3"/>
-        <v>9.1288092963805592E-2</v>
-      </c>
-      <c r="G25" s="5">
-        <f t="shared" si="2"/>
-        <v>0.33845847445658894</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
+        <f>C2*$L$36*(1-C21)</f>
+        <v>842.08</v>
+      </c>
+      <c r="D25" s="6">
+        <f>D2*$L$36*(1-D21)</f>
+        <v>897.18000000000006</v>
+      </c>
+      <c r="E25" s="6">
+        <f>E2*$L$36*(1-E21)</f>
+        <v>766.84</v>
+      </c>
+      <c r="F25" s="6">
+        <f>F2*$L$36*(1-F21)</f>
+        <v>945.06000000000006</v>
+      </c>
+      <c r="G25" s="5"/>
       <c r="H25" s="6"/>
       <c r="L25">
         <v>217</v>
@@ -1075,72 +1026,254 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B26">
-        <f>B25*$L$25</f>
-        <v>2.387</v>
-      </c>
-      <c r="C26" s="9">
-        <f>C25*$L$25</f>
-        <v>15.32450857991784</v>
-      </c>
-      <c r="D26" s="9">
-        <f t="shared" ref="C26:F26" si="4">D25*$L$25</f>
-        <v>19.773366982226484</v>
-      </c>
-      <c r="E26" s="9">
-        <f t="shared" si="4"/>
-        <v>16.151097221789662</v>
-      </c>
-      <c r="F26" s="9">
-        <f t="shared" si="4"/>
-        <v>19.809516173145813</v>
-      </c>
-      <c r="G26" s="11">
-        <f t="shared" si="2"/>
-        <v>73.445488957079803</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <f>($L$32+$L$34)*(D2*$L$28)</f>
+        <v>396.64800000000002</v>
+      </c>
+      <c r="E26" s="6">
+        <f>($L$32+$L$34)*(E2*$L$28)</f>
+        <v>339.024</v>
+      </c>
+      <c r="F26" s="6">
+        <f>($L$32+$L$34)*(F2*$L$28)</f>
+        <v>417.81600000000003</v>
+      </c>
+      <c r="G26" s="11"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <f>(1-B23)*B2+B26</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
+        <f>(1-D23)*D2+D26 - D25</f>
+        <v>1860.4680000000001</v>
+      </c>
+      <c r="E27" s="6">
+        <f>(1-E23)*E2+E26 - E25</f>
+        <v>201.12733333333324</v>
+      </c>
+      <c r="F27" s="6">
+        <f>(1-F23)*F2+F26 - F25</f>
+        <v>1959.7559999999999</v>
+      </c>
       <c r="H27" s="5"/>
       <c r="L27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2">
+        <f>B25*$L$2*$N$2</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" ref="C28:F28" si="5">C25*$L$2*$N$2</f>
+        <v>9.53188540328E-4</v>
+      </c>
+      <c r="D28" s="2">
+        <f>D25*$L$2*$N$2</f>
+        <v>1.015558729113E-3</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="5"/>
+        <v>8.6802097219399995E-4</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="5"/>
+        <v>1.069756272471E-3</v>
+      </c>
       <c r="H28" s="9"/>
       <c r="L28" s="10">
         <v>0.42</v>
       </c>
     </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2">
+        <f>B27*$L$2*$N$2</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" ref="C29:F29" si="6">C27*$L$2*$N$2</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1059481014238002E-3</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="6"/>
+        <v>2.2766514972456656E-4</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="6"/>
+        <v>2.2183366913345998E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="12">
+        <f>B24/B33</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="12">
+        <f t="shared" ref="C30:F30" si="7">C24/C33</f>
+        <v>0.98650254184840658</v>
+      </c>
+      <c r="D30" s="12">
+        <f t="shared" si="7"/>
+        <v>0.96574346782541665</v>
+      </c>
+      <c r="E30" s="12">
+        <f t="shared" si="7"/>
+        <v>0.98527877795599184</v>
+      </c>
+      <c r="F30" s="12">
+        <f t="shared" si="7"/>
+        <v>0.9639811408360861</v>
+      </c>
+    </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="12">
+        <f>B28/B33</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="12">
+        <f>C28/C33</f>
+        <v>1.3497458151593462E-2</v>
+      </c>
+      <c r="D31" s="12">
+        <f>D28/D33</f>
+        <v>1.1145104645840473E-2</v>
+      </c>
+      <c r="E31" s="12">
+        <f>E28/E33</f>
+        <v>1.1662399673501947E-2</v>
+      </c>
+      <c r="F31" s="12">
+        <f>F28/F33</f>
+        <v>1.171846445401311E-2</v>
+      </c>
       <c r="L31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="12">
+        <f>B29/B33</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="12">
+        <f t="shared" ref="C32:F32" si="8">C29/C33</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="12">
+        <f t="shared" si="8"/>
+        <v>2.3111427528742876E-2</v>
+      </c>
+      <c r="E32" s="12">
+        <f t="shared" si="8"/>
+        <v>3.0588223705062113E-3</v>
+      </c>
+      <c r="F32" s="12">
+        <f t="shared" si="8"/>
+        <v>2.4300394709900867E-2</v>
+      </c>
       <c r="L32" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="2">
+        <f>B24+(B25+B27)*$L$2*$N$2</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C33" s="2">
+        <f>C24+(C25+C27)*$L$2*$N$2</f>
+        <v>7.0619855206994653E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <f>D24+(D25+D27)*$L$2*$N$2</f>
+        <v>9.1121506830536797E-2</v>
+      </c>
+      <c r="E33" s="2">
+        <f>E24+(E25+E27)*$L$2*$N$2</f>
+        <v>7.4429019455251905E-2</v>
+      </c>
+      <c r="F33" s="2">
+        <f>F24+(F25+F27)*$L$2*$N$2</f>
+        <v>9.1288092963805592E-2</v>
+      </c>
       <c r="L33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <f>B33*$L$25</f>
+        <v>2.387</v>
+      </c>
+      <c r="C34" s="9">
+        <f>C33*$L$25</f>
+        <v>15.32450857991784</v>
+      </c>
+      <c r="D34" s="9">
+        <f t="shared" ref="D34:F34" si="9">D33*$L$25</f>
+        <v>19.773366982226484</v>
+      </c>
+      <c r="E34" s="9">
+        <f t="shared" si="9"/>
+        <v>16.151097221789662</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="9"/>
+        <v>19.809516173145813</v>
+      </c>
       <c r="L34" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L36" s="8">
         <v>0.38</v>
       </c>

</xml_diff>